<commit_message>
Config File Update 5/6/24
</commit_message>
<xml_diff>
--- a/computingTechnology/computingTechnologyConfig/computingTechnology_CategoryInfo.xlsx
+++ b/computingTechnology/computingTechnologyConfig/computingTechnology_CategoryInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kensch\Box\10. Enterprise Applications\RT-Root\RT-Folders\RT-Config-and-Form-Data\NEW myUMBC Support-RT-Dev-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8929467-7EFD-4D3E-A7CF-05D047DD2DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE7F30-9388-411B-A7E9-944A87A19139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25335" yWindow="-525" windowWidth="21600" windowHeight="11295" xr2:uid="{27652783-9591-D547-A61D-838C8737DB69}"/>
+    <workbookView xWindow="11955" yWindow="4545" windowWidth="21600" windowHeight="11295" xr2:uid="{27652783-9591-D547-A61D-838C8737DB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="290">
   <si>
     <t>Request Type Category</t>
   </si>
@@ -478,9 +478,6 @@
     <t>https://umbc.atlassian.net/wiki/spaces/faq/pages/30744944/What+should+I+do+if+I+receive+a+suspicious+email</t>
   </si>
   <si>
-    <t>How do I subscribe to DoIT IT Security Articles?</t>
-  </si>
-  <si>
     <t>https://umbc.atlassian.net/wiki/spaces/faq/pages/30760620/How+to+Subscribe+to+DoIT+IT+Security+Notices+and+Articles</t>
   </si>
   <si>
@@ -935,6 +932,24 @@
   </si>
   <si>
     <t>Audio Visual Services</t>
+  </si>
+  <si>
+    <t>IT Security</t>
+  </si>
+  <si>
+    <t>What are some Cybersecurity best practices?</t>
+  </si>
+  <si>
+    <t>https://umbc.atlassian.net/wiki/spaces/faq/pages/275611666/What+are+some+Cybersecurity+best+practices</t>
+  </si>
+  <si>
+    <t>What is Duo Multi-Factor Authentication?</t>
+  </si>
+  <si>
+    <t>How can I follow DoIT Security?</t>
+  </si>
+  <si>
+    <t>https://umbc.atlassian.net/wiki/spaces/faq/pages/277774378/What+is+DUO+Multi-Factor+Authentication</t>
   </si>
 </sst>
 </file>
@@ -1389,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0317E7B2-0780-144D-BE4D-E00A0AB6B832}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2327,8 +2342,8 @@
       <c r="A55" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>129</v>
+      <c r="B55" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>130</v>
@@ -2345,16 +2360,16 @@
         <v>129</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>129</v>
+        <v>284</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>132</v>
+        <v>285</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>133</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2362,1323 +2377,1357 @@
         <v>129</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>129</v>
+        <v>284</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>134</v>
+        <v>287</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>135</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>138</v>
+        <v>288</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>137</v>
+        <v>284</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="D60" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="C62" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="5" t="s">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="D65" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="8" t="s">
+      <c r="C66" s="7" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="7" t="s">
+      <c r="D66" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="8" t="s">
+    </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B65" s="6" t="s">
+      <c r="C67" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="5" t="s">
+    </row>
+    <row r="68" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="D68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="5" t="s">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C67" s="7" t="s">
+      <c r="D69" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E67" s="8" t="s">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C70" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="D70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="8" t="s">
+    </row>
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="D71" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B72" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="D72" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C75" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="5" t="s">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C76" s="7" t="s">
+      <c r="D78" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E76" s="8" t="s">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C77" s="7" t="s">
+      <c r="D79" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B80" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="D80" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D84" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E84" s="5" t="s">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="7" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C85" s="7" t="s">
+      <c r="D87" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E85" s="7" t="s">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B86" s="7" t="s">
+      <c r="C88" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="D88" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="D89" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>284</v>
+        <v>200</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>213</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>219</v>
+        <v>21</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="5" t="s">
-        <v>213</v>
+      <c r="E98" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>219</v>
+        <v>21</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="5" t="s">
-        <v>225</v>
+      <c r="E103" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="C104" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>226</v>
-      </c>
       <c r="D104" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="C105" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E107" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E107" s="7" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B108" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>234</v>
+      <c r="C108" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B109" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B109" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E111" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E110" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B112" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C112" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C112" s="5" t="s">
-        <v>243</v>
-      </c>
       <c r="D112" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>249</v>
+        <v>219</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B117" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C117" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="C117" s="5" t="s">
-        <v>254</v>
-      </c>
       <c r="D117" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>115</v>
+        <v>251</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>249</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>257</v>
+        <v>253</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>259</v>
+        <v>219</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>260</v>
+        <v>115</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>259</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>263</v>
+        <v>255</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B122" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="C122" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C122" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="D122" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B123" s="5" t="s">
-        <v>259</v>
-      </c>
       <c r="C123" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B124" s="5" t="s">
-        <v>259</v>
-      </c>
       <c r="C124" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="125" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B125" s="6" t="s">
-        <v>258</v>
-      </c>
       <c r="C125" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>258</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>257</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C130" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E132" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="D130" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E130" s="5" t="s">
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C131" s="1" t="s">
+      <c r="D133" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>283</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E130">
-    <sortCondition ref="A2:A130"/>
-    <sortCondition ref="B2:B130"/>
-    <sortCondition ref="C2:C130"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E132">
+    <sortCondition ref="A2:A132"/>
+    <sortCondition ref="B2:B132"/>
+    <sortCondition ref="C2:C132"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="E30" r:id="rId1" xr:uid="{D0455084-24A5-43EA-843F-C3AA684FF9C8}"/>
     <hyperlink ref="E13" r:id="rId2" xr:uid="{24374FBC-1F6B-46FC-B613-51157541814D}"/>
-    <hyperlink ref="E75" r:id="rId3" xr:uid="{DC8A4600-DE0B-4F8A-8CA6-6942CDF029B4}"/>
-    <hyperlink ref="E73" r:id="rId4" xr:uid="{79583B20-ACEE-4A1C-BA07-F8FBD2543B9B}"/>
-    <hyperlink ref="E76" r:id="rId5" xr:uid="{FBA6B573-0670-498F-8319-0997EA9BC393}"/>
-    <hyperlink ref="E70" r:id="rId6" xr:uid="{B4F6A97F-7325-4FB5-9DF8-CE8C30121699}"/>
-    <hyperlink ref="E58" r:id="rId7" xr:uid="{DB1F644F-29D0-4A2B-A499-15D45755040B}"/>
-    <hyperlink ref="E60" r:id="rId8" xr:uid="{840B3C73-8096-4BE7-9D32-6588180A6A95}"/>
-    <hyperlink ref="E63" r:id="rId9" xr:uid="{2E872EBF-01C5-431E-AEB6-A5E5F747E962}"/>
-    <hyperlink ref="E64" r:id="rId10" xr:uid="{D01F6FF4-DCD6-4FCA-8817-1B361A27B4EF}"/>
-    <hyperlink ref="E69" r:id="rId11" xr:uid="{D8692531-8B79-4D78-82EC-17FE30B6485D}"/>
-    <hyperlink ref="E79" r:id="rId12" xr:uid="{72BC75DE-308A-48FE-8AC6-863A46789801}"/>
-    <hyperlink ref="E80" r:id="rId13" xr:uid="{E9B671A8-3D19-47C3-9528-5FF76FD4AA0C}"/>
-    <hyperlink ref="E81" r:id="rId14" xr:uid="{EC469E29-9D97-4815-A7F9-04536F357351}"/>
-    <hyperlink ref="E82" r:id="rId15" xr:uid="{8138F5B3-2B69-4D99-8C3C-41B12479ABDE}"/>
-    <hyperlink ref="E83" r:id="rId16" xr:uid="{34413946-9B1B-494F-B8C8-A7B8F62E743E}"/>
-    <hyperlink ref="E84" r:id="rId17" xr:uid="{8657BEB7-B585-46E4-B726-257DD978EA6F}"/>
-    <hyperlink ref="E78" r:id="rId18" xr:uid="{1A878E81-4126-45A5-BF26-6ED850BFEBF5}"/>
-    <hyperlink ref="E91" r:id="rId19" xr:uid="{D7A8CDEF-1791-4570-8CC4-F531DB1E34F5}"/>
-    <hyperlink ref="E67" r:id="rId20" xr:uid="{E1C2DA3A-2CAA-48BC-98ED-292D2DBFE10B}"/>
+    <hyperlink ref="E77" r:id="rId3" xr:uid="{DC8A4600-DE0B-4F8A-8CA6-6942CDF029B4}"/>
+    <hyperlink ref="E75" r:id="rId4" xr:uid="{79583B20-ACEE-4A1C-BA07-F8FBD2543B9B}"/>
+    <hyperlink ref="E78" r:id="rId5" xr:uid="{FBA6B573-0670-498F-8319-0997EA9BC393}"/>
+    <hyperlink ref="E72" r:id="rId6" xr:uid="{B4F6A97F-7325-4FB5-9DF8-CE8C30121699}"/>
+    <hyperlink ref="E60" r:id="rId7" xr:uid="{DB1F644F-29D0-4A2B-A499-15D45755040B}"/>
+    <hyperlink ref="E62" r:id="rId8" xr:uid="{840B3C73-8096-4BE7-9D32-6588180A6A95}"/>
+    <hyperlink ref="E65" r:id="rId9" xr:uid="{2E872EBF-01C5-431E-AEB6-A5E5F747E962}"/>
+    <hyperlink ref="E66" r:id="rId10" xr:uid="{D01F6FF4-DCD6-4FCA-8817-1B361A27B4EF}"/>
+    <hyperlink ref="E71" r:id="rId11" xr:uid="{D8692531-8B79-4D78-82EC-17FE30B6485D}"/>
+    <hyperlink ref="E81" r:id="rId12" xr:uid="{72BC75DE-308A-48FE-8AC6-863A46789801}"/>
+    <hyperlink ref="E82" r:id="rId13" xr:uid="{E9B671A8-3D19-47C3-9528-5FF76FD4AA0C}"/>
+    <hyperlink ref="E83" r:id="rId14" xr:uid="{EC469E29-9D97-4815-A7F9-04536F357351}"/>
+    <hyperlink ref="E84" r:id="rId15" xr:uid="{8138F5B3-2B69-4D99-8C3C-41B12479ABDE}"/>
+    <hyperlink ref="E85" r:id="rId16" xr:uid="{34413946-9B1B-494F-B8C8-A7B8F62E743E}"/>
+    <hyperlink ref="E86" r:id="rId17" xr:uid="{8657BEB7-B585-46E4-B726-257DD978EA6F}"/>
+    <hyperlink ref="E80" r:id="rId18" xr:uid="{1A878E81-4126-45A5-BF26-6ED850BFEBF5}"/>
+    <hyperlink ref="E93" r:id="rId19" xr:uid="{D7A8CDEF-1791-4570-8CC4-F531DB1E34F5}"/>
+    <hyperlink ref="E69" r:id="rId20" xr:uid="{E1C2DA3A-2CAA-48BC-98ED-292D2DBFE10B}"/>
     <hyperlink ref="E41" r:id="rId21" xr:uid="{66F5B276-B76C-4A01-9921-70EAE15F6671}"/>
     <hyperlink ref="E31" r:id="rId22" xr:uid="{96594008-D2AB-4743-AD6C-E16870AE8F18}"/>
     <hyperlink ref="E5" r:id="rId23" xr:uid="{2597498E-3741-5B48-A389-F950F1C4255E}"/>
     <hyperlink ref="E9" r:id="rId24" xr:uid="{EE3AD498-C6C7-F241-B3E9-07161A91423D}"/>
-    <hyperlink ref="E56" r:id="rId25" xr:uid="{3C1FCCA2-77EA-9641-A69D-0F5CAF34C208}"/>
-    <hyperlink ref="E109" r:id="rId26" xr:uid="{9AB60516-2C05-1449-ABFB-C4A67B553A2E}"/>
-    <hyperlink ref="E111" r:id="rId27" xr:uid="{3F8A57FC-E783-4145-82F7-6E11DA93588D}"/>
+    <hyperlink ref="E58" r:id="rId25" xr:uid="{3C1FCCA2-77EA-9641-A69D-0F5CAF34C208}"/>
+    <hyperlink ref="E111" r:id="rId26" xr:uid="{9AB60516-2C05-1449-ABFB-C4A67B553A2E}"/>
+    <hyperlink ref="E113" r:id="rId27" xr:uid="{3F8A57FC-E783-4145-82F7-6E11DA93588D}"/>
     <hyperlink ref="E14" r:id="rId28" xr:uid="{100D5DCF-52D4-49D2-9586-95CAB96879C7}"/>
-    <hyperlink ref="E61" r:id="rId29" xr:uid="{0A20DE64-B401-4DD0-9EF4-55E2286F16B5}"/>
-    <hyperlink ref="E62" r:id="rId30" xr:uid="{0F0E21DF-421D-4C89-837D-A5E1D2296908}"/>
-    <hyperlink ref="E59" r:id="rId31" xr:uid="{C2780FD5-A2C5-4A39-85DC-3BDF8F1EA3C1}"/>
-    <hyperlink ref="E87" r:id="rId32" xr:uid="{F902BFDF-B9DC-4E8D-B42F-083EB0FA0458}"/>
-    <hyperlink ref="E89" r:id="rId33" xr:uid="{9DBE9EAC-DCCA-44EF-840A-D4CCDF3778DA}"/>
-    <hyperlink ref="E92" r:id="rId34" xr:uid="{B27CFD74-AB38-4D59-BD69-1C7334042FF4}"/>
-    <hyperlink ref="E93" r:id="rId35" xr:uid="{B5275E16-F27A-4BB0-B765-75CF5F64F966}"/>
-    <hyperlink ref="E97" r:id="rId36" xr:uid="{0460510B-4A4D-024A-BC03-EFACA17D3AB9}"/>
-    <hyperlink ref="E98" r:id="rId37" xr:uid="{6CCD9E3A-7AF0-FA4E-854D-C29671AF4876}"/>
-    <hyperlink ref="E77" r:id="rId38" xr:uid="{8B6F3663-F167-485B-AA3B-989A47265C7B}"/>
-    <hyperlink ref="E96" r:id="rId39" xr:uid="{FD9888E8-CBB9-49DE-B4CC-5C10DD2F5348}"/>
-    <hyperlink ref="E101" r:id="rId40" xr:uid="{B335141E-7959-4A8D-A936-AB25F00C3059}"/>
+    <hyperlink ref="E63" r:id="rId29" xr:uid="{0A20DE64-B401-4DD0-9EF4-55E2286F16B5}"/>
+    <hyperlink ref="E64" r:id="rId30" xr:uid="{0F0E21DF-421D-4C89-837D-A5E1D2296908}"/>
+    <hyperlink ref="E61" r:id="rId31" xr:uid="{C2780FD5-A2C5-4A39-85DC-3BDF8F1EA3C1}"/>
+    <hyperlink ref="E89" r:id="rId32" xr:uid="{F902BFDF-B9DC-4E8D-B42F-083EB0FA0458}"/>
+    <hyperlink ref="E91" r:id="rId33" xr:uid="{9DBE9EAC-DCCA-44EF-840A-D4CCDF3778DA}"/>
+    <hyperlink ref="E94" r:id="rId34" xr:uid="{B27CFD74-AB38-4D59-BD69-1C7334042FF4}"/>
+    <hyperlink ref="E95" r:id="rId35" xr:uid="{B5275E16-F27A-4BB0-B765-75CF5F64F966}"/>
+    <hyperlink ref="E99" r:id="rId36" xr:uid="{0460510B-4A4D-024A-BC03-EFACA17D3AB9}"/>
+    <hyperlink ref="E100" r:id="rId37" xr:uid="{6CCD9E3A-7AF0-FA4E-854D-C29671AF4876}"/>
+    <hyperlink ref="E79" r:id="rId38" xr:uid="{8B6F3663-F167-485B-AA3B-989A47265C7B}"/>
+    <hyperlink ref="E98" r:id="rId39" xr:uid="{FD9888E8-CBB9-49DE-B4CC-5C10DD2F5348}"/>
+    <hyperlink ref="E103" r:id="rId40" xr:uid="{B335141E-7959-4A8D-A936-AB25F00C3059}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId41"/>

</xml_diff>